<commit_message>
All tabs withing stats page created
</commit_message>
<xml_diff>
--- a/bug-report.xlsx
+++ b/bug-report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Projects\footstats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2877D50-8173-4E29-B7C0-20E81F905A0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB3426F9-3437-4A7A-A766-FEE27A6D29BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="28">
   <si>
     <t>Bug ID</t>
   </si>
@@ -97,6 +97,18 @@
   </si>
   <si>
     <t>logo is not proper.</t>
+  </si>
+  <si>
+    <t>05.stats.tabs</t>
+  </si>
+  <si>
+    <t>Tabs are not switching properly on reload and on clicking</t>
+  </si>
+  <si>
+    <t>the stats navbar link</t>
+  </si>
+  <si>
+    <t>home-&gt;statspage-&gt;tabs</t>
   </si>
 </sst>
 </file>
@@ -443,10 +455,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T13"/>
+  <dimension ref="A1:T16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q23" sqref="Q23:R23"/>
+      <selection activeCell="Q20" sqref="Q20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -556,6 +568,28 @@
         <v>23</v>
       </c>
     </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" t="s">
+        <v>25</v>
+      </c>
+      <c r="J15" t="s">
+        <v>27</v>
+      </c>
+      <c r="O15" t="s">
+        <v>15</v>
+      </c>
+      <c r="T15" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="D16" t="s">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>